<commit_message>
Verified working with new products
</commit_message>
<xml_diff>
--- a/input/370.xlsx
+++ b/input/370.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="66">
   <si>
     <t>Product History</t>
   </si>
@@ -21,7 +21,7 @@
     <t>Product</t>
   </si>
   <si>
-    <t>AWP01</t>
+    <t>MD01</t>
   </si>
   <si>
     <t>Store</t>
@@ -78,22 +78,130 @@
     <t>Last Changed Time</t>
   </si>
   <si>
+    <t>INVC</t>
+  </si>
+  <si>
+    <t>3700006923</t>
+  </si>
+  <si>
+    <t>SOUTHERN INDIANA SCALE CO</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t xml:space="preserve">U651RHY   </t>
+  </si>
+  <si>
+    <t>13:52:33</t>
+  </si>
+  <si>
+    <t>3700006854</t>
+  </si>
+  <si>
+    <t>MILLERS AUTO BODY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U651JTW   </t>
+  </si>
+  <si>
+    <t>13:27:34</t>
+  </si>
+  <si>
+    <t>3700006520</t>
+  </si>
+  <si>
+    <t>RIVER METALS REC LOU STL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U651CTW   </t>
+  </si>
+  <si>
+    <t>12:39:54</t>
+  </si>
+  <si>
+    <t>15:49:05</t>
+  </si>
+  <si>
+    <t>3700006284</t>
+  </si>
+  <si>
+    <t>ROGERS GROUP (KY)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U651MCB   </t>
+  </si>
+  <si>
+    <t>12:10:58</t>
+  </si>
+  <si>
     <t>VINV</t>
   </si>
   <si>
-    <t>3700003061</t>
+    <t>13720</t>
   </si>
   <si>
     <t>VOID</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t xml:space="preserve">U651RLW   </t>
-  </si>
-  <si>
-    <t>10:07:56</t>
+    <t>3700006212</t>
+  </si>
+  <si>
+    <t>RIVER METALS REC - NEWPOR</t>
+  </si>
+  <si>
+    <t>07:44:53</t>
+  </si>
+  <si>
+    <t>3700006152</t>
+  </si>
+  <si>
+    <t>12:14:05</t>
+  </si>
+  <si>
+    <t>11:25:38</t>
+  </si>
+  <si>
+    <t>3700005942</t>
+  </si>
+  <si>
+    <t>LEHIGH HANSON-CEMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U651JPW   </t>
+  </si>
+  <si>
+    <t>23:15:59</t>
+  </si>
+  <si>
+    <t>3700005883</t>
+  </si>
+  <si>
+    <t>08:55:58</t>
+  </si>
+  <si>
+    <t>09:56:08</t>
+  </si>
+  <si>
+    <t>3700005867</t>
+  </si>
+  <si>
+    <t>08:53:25</t>
+  </si>
+  <si>
+    <t>10:25:08</t>
+  </si>
+  <si>
+    <t>3700005882</t>
+  </si>
+  <si>
+    <t>HILLTOP BIG BEND QUARRY</t>
+  </si>
+  <si>
+    <t>08:45:55</t>
+  </si>
+  <si>
+    <t>09:46:04</t>
   </si>
   <si>
     <t>Beginning Balance</t>
@@ -158,7 +266,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -251,7 +359,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n" s="2">
-        <v>44624.0</v>
+        <v>45037.0</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -260,7 +368,7 @@
         <v>22</v>
       </c>
       <c r="D5" t="n">
-        <v>2857412.0</v>
+        <v>2857604.0</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
@@ -272,19 +380,19 @@
         <v>0.0</v>
       </c>
       <c r="H5" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="I5" t="n">
-        <v>75.0</v>
+        <v>45.0</v>
       </c>
       <c r="J5" t="n">
-        <v>50.0</v>
+        <v>37.5</v>
       </c>
       <c r="K5" t="n">
         <v>0.0</v>
       </c>
       <c r="L5" t="n" s="2">
-        <v>44624.0</v>
+        <v>45037.0</v>
       </c>
       <c r="M5" t="s">
         <v>21</v>
@@ -296,7 +404,7 @@
         <v>25</v>
       </c>
       <c r="P5" t="n" s="2">
-        <v>44624.0</v>
+        <v>45037.0</v>
       </c>
       <c r="Q5" t="s">
         <v>26</v>
@@ -305,33 +413,653 @@
         <v>25</v>
       </c>
       <c r="S5" t="n" s="2">
-        <v>44624.0</v>
+        <v>45037.0</v>
       </c>
       <c r="T5" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n" s="2">
+        <v>45030.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="n">
+        <v>370.0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L6" t="n" s="2">
+        <v>45030.0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P6" t="n" s="2">
+        <v>45030.0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>30</v>
+      </c>
+      <c r="R6" t="s">
+        <v>29</v>
+      </c>
+      <c r="S6" t="n" s="2">
+        <v>45030.0</v>
+      </c>
+      <c r="T6" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="7">
-      <c r="E7" t="s" s="1">
-        <v>27</v>
-      </c>
-      <c r="F7" t="n" s="1">
-        <v>0.0</v>
+      <c r="A7" t="n" s="2">
+        <v>44999.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2855395.0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L7" t="n" s="2">
+        <v>44999.0</v>
+      </c>
+      <c r="M7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O7" t="s">
+        <v>33</v>
+      </c>
+      <c r="P7" t="n" s="2">
+        <v>44974.0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R7" t="s">
+        <v>33</v>
+      </c>
+      <c r="S7" t="n" s="2">
+        <v>44999.0</v>
+      </c>
+      <c r="T7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8">
-      <c r="E8" t="s" s="1">
-        <v>28</v>
-      </c>
-      <c r="F8" t="n" s="1">
-        <v>0.0</v>
+      <c r="A8" t="n" s="2">
+        <v>44977.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2857036.0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-3.0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L8" t="n" s="2">
+        <v>44977.0</v>
+      </c>
+      <c r="M8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" t="s">
+        <v>36</v>
+      </c>
+      <c r="O8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P8" t="n" s="2">
+        <v>44977.0</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>39</v>
+      </c>
+      <c r="R8" t="s">
+        <v>38</v>
+      </c>
+      <c r="S8" t="n" s="2">
+        <v>44977.0</v>
+      </c>
+      <c r="T8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9">
-      <c r="E9" t="s" s="1">
-        <v>29</v>
-      </c>
-      <c r="F9" t="n" s="1">
+      <c r="A9" t="n" s="2">
+        <v>44974.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2855395.0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L9" t="n" s="2">
+        <v>44974.0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" t="s">
+        <v>33</v>
+      </c>
+      <c r="P9" t="n" s="2">
+        <v>44974.0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>34</v>
+      </c>
+      <c r="R9" t="s">
+        <v>33</v>
+      </c>
+      <c r="S9" t="n" s="2">
+        <v>44974.0</v>
+      </c>
+      <c r="T9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n" s="2">
+        <v>44967.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2855395.0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="J10" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L10" t="n" s="2">
+        <v>44967.0</v>
+      </c>
+      <c r="M10" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" t="s">
+        <v>43</v>
+      </c>
+      <c r="O10" t="s">
+        <v>33</v>
+      </c>
+      <c r="P10" t="n" s="2">
+        <v>44967.0</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>45</v>
+      </c>
+      <c r="R10" t="s">
+        <v>33</v>
+      </c>
+      <c r="S10" t="n" s="2">
+        <v>44967.0</v>
+      </c>
+      <c r="T10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n" s="2">
+        <v>44966.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2857036.0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L11" t="n" s="2">
+        <v>44966.0</v>
+      </c>
+      <c r="M11" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" t="s">
+        <v>46</v>
+      </c>
+      <c r="O11" t="s">
+        <v>38</v>
+      </c>
+      <c r="P11" t="n" s="2">
+        <v>44960.0</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>47</v>
+      </c>
+      <c r="R11" t="s">
+        <v>38</v>
+      </c>
+      <c r="S11" t="n" s="2">
+        <v>44966.0</v>
+      </c>
+      <c r="T11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n" s="2">
+        <v>44942.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2852297.0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L12" t="n" s="2">
+        <v>44942.0</v>
+      </c>
+      <c r="M12" t="s">
+        <v>21</v>
+      </c>
+      <c r="N12" t="s">
+        <v>49</v>
+      </c>
+      <c r="O12" t="s">
+        <v>51</v>
+      </c>
+      <c r="P12" t="n" s="2">
+        <v>44936.0</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>52</v>
+      </c>
+      <c r="R12" t="s">
+        <v>51</v>
+      </c>
+      <c r="S12" t="n" s="2">
+        <v>44936.0</v>
+      </c>
+      <c r="T12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n" s="2">
+        <v>44932.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2857036.0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L13" t="n" s="2">
+        <v>44932.0</v>
+      </c>
+      <c r="M13" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" t="s">
+        <v>53</v>
+      </c>
+      <c r="O13" t="s">
+        <v>38</v>
+      </c>
+      <c r="P13" t="n" s="2">
+        <v>44931.0</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>54</v>
+      </c>
+      <c r="R13" t="s">
+        <v>38</v>
+      </c>
+      <c r="S13" t="n" s="2">
+        <v>44931.0</v>
+      </c>
+      <c r="T13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n" s="2">
+        <v>44932.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2857036.0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L14" t="n" s="2">
+        <v>44932.0</v>
+      </c>
+      <c r="M14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" t="s">
+        <v>56</v>
+      </c>
+      <c r="O14" t="s">
+        <v>38</v>
+      </c>
+      <c r="P14" t="n" s="2">
+        <v>44930.0</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>57</v>
+      </c>
+      <c r="R14" t="s">
+        <v>38</v>
+      </c>
+      <c r="S14" t="n" s="2">
+        <v>44931.0</v>
+      </c>
+      <c r="T14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n" s="2">
+        <v>44931.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2852994.0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L15" t="n" s="2">
+        <v>44931.0</v>
+      </c>
+      <c r="M15" t="s">
+        <v>21</v>
+      </c>
+      <c r="N15" t="s">
+        <v>59</v>
+      </c>
+      <c r="O15" t="s">
+        <v>38</v>
+      </c>
+      <c r="P15" t="n" s="2">
+        <v>44931.0</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>61</v>
+      </c>
+      <c r="R15" t="s">
+        <v>38</v>
+      </c>
+      <c r="S15" t="n" s="2">
+        <v>44931.0</v>
+      </c>
+      <c r="T15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="E17" t="s" s="1">
+        <v>63</v>
+      </c>
+      <c r="F17" t="n" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="E18" t="s" s="1">
+        <v>64</v>
+      </c>
+      <c r="F18" t="n" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="E19" t="s" s="1">
+        <v>65</v>
+      </c>
+      <c r="F19" t="n" s="1">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>